<commit_message>
q3 post-deflators adj and post-mpi
</commit_message>
<xml_diff>
--- a/results/12-2022/comparison-deflators-12-2022.xlsx
+++ b/results/12-2022/comparison-deflators-12-2022.xlsx
@@ -566,7 +566,7 @@
         <v>0.0106</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0068</v>
+        <v>0.0082</v>
       </c>
       <c r="J2" t="n">
         <v>0.0062</v>
@@ -672,10 +672,10 @@
         <v>0.0247</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.0364</v>
+        <v>-0.0365</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.0353</v>
+        <v>-0.0354</v>
       </c>
       <c r="K4" t="n">
         <v>-0.0006</v>
@@ -687,16 +687,16 @@
         <v>-0.0074</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0072</v>
+        <v>-0.0073</v>
       </c>
       <c r="O4" t="n">
         <v>-0.0179</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0686</v>
+        <v>-0.0687</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.0298</v>
+        <v>-0.0299</v>
       </c>
     </row>
     <row r="5">
@@ -725,10 +725,10 @@
         <v>-0.1874</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.2155</v>
+        <v>-0.1777</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.3575</v>
+        <v>-0.4306</v>
       </c>
       <c r="K5" t="n">
         <v>-0.0642</v>
@@ -778,31 +778,31 @@
         <v>-0.0515</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.059</v>
+        <v>-0.0587</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0855</v>
+        <v>-0.0852</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.0917</v>
+        <v>-0.0915</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.0763</v>
+        <v>-0.076</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0728</v>
+        <v>-0.0726</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0627</v>
+        <v>-0.0625</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.0494</v>
+        <v>-0.0492</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0531</v>
+        <v>-0.0529</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.034</v>
+        <v>-0.0338</v>
       </c>
     </row>
     <row r="7">
@@ -831,31 +831,31 @@
         <v>-0.0883</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.0582</v>
+        <v>-0.0735</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0688</v>
+        <v>-0.0839</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0785</v>
+        <v>0.0636</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.0216</v>
+        <v>-0.0358</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.022</v>
+        <v>-0.0213</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.0467</v>
+        <v>-0.0458</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0716</v>
+        <v>-0.0706</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0343</v>
+        <v>0.0349</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0328</v>
+        <v>0.0334</v>
       </c>
     </row>
     <row r="8">
@@ -884,31 +884,31 @@
         <v>-0.5595</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.4981</v>
+        <v>-0.453</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.2469</v>
+        <v>-0.2229</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0942</v>
+        <v>-0.0924</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0797</v>
+        <v>-0.0679</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0171</v>
+        <v>0.0287</v>
       </c>
       <c r="N8" t="n">
-        <v>0.3157</v>
+        <v>0.3272</v>
       </c>
       <c r="O8" t="n">
-        <v>0.3096</v>
+        <v>0.321</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3269</v>
+        <v>0.3382</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.3548</v>
+        <v>0.3453</v>
       </c>
     </row>
     <row r="9">
@@ -937,28 +937,28 @@
         <v>-0.1402</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.1017</v>
+        <v>-0.0907</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0591</v>
+        <v>-0.0624</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0386</v>
+        <v>-0.0388</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0118</v>
+        <v>-0.0157</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0177</v>
+        <v>-0.0178</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0393</v>
+        <v>-0.0394</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0343</v>
+        <v>-0.0344</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0283</v>
+        <v>-0.0284</v>
       </c>
       <c r="Q9" t="n">
         <v>-0.0189</v>
@@ -990,19 +990,19 @@
         <v>0.0493</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.0924</v>
+        <v>-0.0927</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.0805</v>
+        <v>-0.0806</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.0937</v>
+        <v>-0.0939</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.0926</v>
+        <v>-0.0927</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.0816</v>
+        <v>-0.0817</v>
       </c>
       <c r="N10" t="n">
         <v>-0.0522</v>
@@ -1043,7 +1043,7 @@
         <v>0.0118</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0058</v>
+        <v>0.0071</v>
       </c>
       <c r="J11" t="n">
         <v>0.0054</v>
@@ -1096,16 +1096,16 @@
         <v>-0.8494</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.5856</v>
+        <v>-0.5943</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.1346</v>
+        <v>-0.1432</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.0089</v>
+        <v>-0.0174</v>
       </c>
       <c r="L12" t="n">
-        <v>0.054</v>
+        <v>0.0456</v>
       </c>
       <c r="M12" t="n">
         <v>-0.0449</v>
@@ -1202,31 +1202,31 @@
         <v>-0.084</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.0735</v>
+        <v>-0.0708</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.0583</v>
+        <v>-0.0589</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.5231</v>
+        <v>-0.5233</v>
       </c>
       <c r="L14" t="n">
-        <v>-0.5714</v>
+        <v>-0.5717</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.2219</v>
+        <v>-0.2222</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.1757</v>
+        <v>-0.1758</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.3205</v>
+        <v>-0.3206</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2398</v>
+        <v>-0.2399</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.103</v>
+        <v>-0.1032</v>
       </c>
     </row>
     <row r="15">
@@ -1255,31 +1255,31 @@
         <v>-0.9651</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.3972</v>
+        <v>-0.3956</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.3915</v>
+        <v>-0.3902</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.2846</v>
+        <v>-0.2835</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.1296</v>
+        <v>-0.1285</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.0073</v>
+        <v>-0.0067</v>
       </c>
       <c r="N15" t="n">
-        <v>-0.0012</v>
+        <v>-0.0009</v>
       </c>
       <c r="O15" t="n">
-        <v>-0.0007</v>
+        <v>-0.0002</v>
       </c>
       <c r="P15" t="n">
-        <v>-0.0003</v>
+        <v>0.0001</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="16">
@@ -1308,31 +1308,31 @@
         <v>-2.563</v>
       </c>
       <c r="I16" t="n">
-        <v>-2.104</v>
+        <v>-2.1018</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.8317</v>
+        <v>-1.8326</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.5298</v>
+        <v>-2.5519</v>
       </c>
       <c r="L16" t="n">
-        <v>-1.0486</v>
+        <v>-1.0643</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.4853</v>
+        <v>-0.4702</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.1832</v>
+        <v>-0.1682</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.3832</v>
+        <v>-0.368</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.3535</v>
+        <v>-0.3384</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0013</v>
+        <v>-0.0074</v>
       </c>
     </row>
     <row r="17">
@@ -1414,10 +1414,10 @@
         <v>-0.3044</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.2535</v>
+        <v>-0.1803</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.3491</v>
+        <v>-0.4223</v>
       </c>
       <c r="K18" t="n">
         <v>-0.0362</v>
@@ -1626,10 +1626,10 @@
         <v>0.5029</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2093</v>
+        <v>0.1361</v>
       </c>
       <c r="J22" t="n">
-        <v>0.2821</v>
+        <v>0.3552</v>
       </c>
       <c r="K22" t="n">
         <v>-0.0654</v>
@@ -1679,28 +1679,28 @@
         <v>-0.0058</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.0065</v>
+        <v>-0.0064</v>
       </c>
       <c r="J23" t="n">
         <v>-0.0082</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.0087</v>
+        <v>-0.0086</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.0002</v>
+        <v>-0.0001</v>
       </c>
       <c r="M23" t="n">
         <v>0.0022</v>
       </c>
       <c r="N23" t="n">
-        <v>0.0038</v>
+        <v>0.0039</v>
       </c>
       <c r="O23" t="n">
         <v>0.0046</v>
       </c>
       <c r="P23" t="n">
-        <v>0.0063</v>
+        <v>0.0064</v>
       </c>
       <c r="Q23" t="n">
         <v>0.0133</v>
@@ -1732,31 +1732,31 @@
         <v>-0.1434</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.0753</v>
+        <v>-0.0786</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0081</v>
+        <v>0.0049</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0784</v>
+        <v>-0.0816</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1289</v>
+        <v>0.1253</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1114</v>
+        <v>0.111</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0972</v>
+        <v>0.0968</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0833</v>
+        <v>0.083</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.06</v>
+        <v>-0.0598</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.048</v>
+        <v>-0.0478</v>
       </c>
     </row>
     <row r="25">
@@ -1785,28 +1785,28 @@
         <v>0.0586</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.0016</v>
+        <v>0.004</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.0099</v>
+        <v>-0.0043</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0589</v>
+        <v>0.0616</v>
       </c>
       <c r="L25" t="n">
-        <v>-0.002</v>
+        <v>0.0007</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0168</v>
+        <v>0.0194</v>
       </c>
       <c r="N25" t="n">
-        <v>0.0049</v>
+        <v>0.0075</v>
       </c>
       <c r="O25" t="n">
-        <v>-0.0105</v>
+        <v>-0.0079</v>
       </c>
       <c r="P25" t="n">
-        <v>-0.0177</v>
+        <v>-0.0151</v>
       </c>
       <c r="Q25" t="n">
         <v>0.0032</v>
@@ -2000,13 +2000,13 @@
         <v>-0.0525</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.0402</v>
+        <v>-0.0403</v>
       </c>
       <c r="K29" t="n">
-        <v>-0.0273</v>
+        <v>-0.0274</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.0162</v>
+        <v>-0.0163</v>
       </c>
       <c r="M29" t="n">
         <v>-0.007</v>
@@ -2050,7 +2050,7 @@
         <v>0.0001</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>0.0014</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -2156,10 +2156,10 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -2209,10 +2209,10 @@
         <v>0.0216</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0002</v>
+        <v>0.038</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0003</v>
+        <v>-0.0728</v>
       </c>
       <c r="K33" t="n">
         <v>0.0001</v>
@@ -2262,31 +2262,31 @@
         <v>-0.0031</v>
       </c>
       <c r="I34" t="n">
-        <v>-0.0031</v>
+        <v>-0.0029</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.0031</v>
+        <v>-0.0029</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.0032</v>
+        <v>-0.0029</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.0032</v>
+        <v>-0.003</v>
       </c>
       <c r="M34" t="n">
-        <v>-0.0032</v>
+        <v>-0.003</v>
       </c>
       <c r="N34" t="n">
-        <v>-0.0032</v>
+        <v>-0.003</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0032</v>
+        <v>-0.0029</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.0031</v>
+        <v>-0.0029</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.0031</v>
+        <v>-0.0029</v>
       </c>
     </row>
     <row r="35">
@@ -2315,31 +2315,31 @@
         <v>-0.0007</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.0027</v>
+        <v>-0.0181</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.0047</v>
+        <v>-0.0198</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.0067</v>
+        <v>-0.0216</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.0066</v>
+        <v>-0.0208</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.0045</v>
+        <v>-0.0038</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.0026</v>
+        <v>-0.0017</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.0006</v>
+        <v>0.0004</v>
       </c>
       <c r="P35" t="n">
-        <v>0</v>
+        <v>0.0006</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.0001</v>
+        <v>0.0008</v>
       </c>
     </row>
     <row r="36">
@@ -2368,31 +2368,31 @@
         <v>0.0111</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0112</v>
+        <v>0.0563</v>
       </c>
       <c r="J36" t="n">
-        <v>0.0054</v>
+        <v>0.0294</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0051</v>
+        <v>0.007</v>
       </c>
       <c r="L36" t="n">
-        <v>0.005</v>
+        <v>0.0168</v>
       </c>
       <c r="M36" t="n">
-        <v>0.0048</v>
+        <v>0.0164</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0044</v>
+        <v>0.0159</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0043</v>
+        <v>0.0157</v>
       </c>
       <c r="P36" t="n">
-        <v>-0.0008</v>
+        <v>0.0105</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.0008</v>
+        <v>-0.0104</v>
       </c>
     </row>
     <row r="37">
@@ -2421,19 +2421,19 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>0.0001</v>
+        <v>0.0111</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>-0.0032</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="L37" t="n">
-        <v>0</v>
+        <v>-0.0039</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="N37" t="n">
         <v>0</v>
@@ -2474,19 +2474,19 @@
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="J38" t="n">
-        <v>0.0001</v>
+        <v>-0.0001</v>
       </c>
       <c r="K38" t="n">
-        <v>0.0001</v>
+        <v>-0.0001</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0001</v>
+        <v>-0.0001</v>
       </c>
       <c r="M38" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
@@ -2527,7 +2527,7 @@
         <v>-0.0007</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>0.0014</v>
       </c>
       <c r="J39" t="n">
         <v>0</v>
@@ -2580,16 +2580,16 @@
         <v>-0.0055</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.0055</v>
+        <v>-0.0142</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.0054</v>
+        <v>-0.014</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.0054</v>
+        <v>-0.0139</v>
       </c>
       <c r="L40" t="n">
-        <v>-0.0001</v>
+        <v>-0.0085</v>
       </c>
       <c r="M40" t="n">
         <v>0.0006</v>
@@ -2686,31 +2686,31 @@
         <v>0.0003</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>0.0027</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="K42" t="n">
-        <v>0.0005</v>
+        <v>0.0002</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0005</v>
+        <v>0.0003</v>
       </c>
       <c r="M42" t="n">
+        <v>0</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="O42" t="n">
         <v>0.0002</v>
       </c>
-      <c r="N42" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="O42" t="n">
-        <v>0.0003</v>
-      </c>
       <c r="P42" t="n">
-        <v>0.0002</v>
+        <v>0.0001</v>
       </c>
       <c r="Q42" t="n">
-        <v>0.0001</v>
+        <v>-0.0001</v>
       </c>
     </row>
     <row r="43">
@@ -2739,31 +2739,31 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="J43" t="n">
+        <v>0.0017</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0.0014</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.0006</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="P43" t="n">
         <v>0.0004</v>
       </c>
-      <c r="J43" t="n">
-        <v>0.0004</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="L43" t="n">
+      <c r="Q43" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="n">
-        <v>0</v>
-      </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -2792,31 +2792,31 @@
         <v>0.1415</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0195</v>
+        <v>0.0217</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.005</v>
+        <v>-0.0059</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.0069</v>
+        <v>-0.029</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0084</v>
+        <v>-0.0072</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0111</v>
+        <v>0.0262</v>
       </c>
       <c r="N44" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.0309</v>
+      </c>
+      <c r="P44" t="n">
         <v>0.013</v>
       </c>
-      <c r="O44" t="n">
-        <v>0.0158</v>
-      </c>
-      <c r="P44" t="n">
-        <v>-0.0022</v>
-      </c>
       <c r="Q44" t="n">
-        <v>-0.0024</v>
+        <v>-0.0111</v>
       </c>
     </row>
     <row r="45">
@@ -2898,10 +2898,10 @@
         <v>-0.0007</v>
       </c>
       <c r="I46" t="n">
-        <v>0.0002</v>
+        <v>0.0735</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0003</v>
+        <v>-0.0728</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
@@ -3110,10 +3110,10 @@
         <v>0.0983</v>
       </c>
       <c r="I50" t="n">
-        <v>-0.0003</v>
+        <v>-0.0735</v>
       </c>
       <c r="J50" t="n">
-        <v>-0.0004</v>
+        <v>0.0727</v>
       </c>
       <c r="K50" t="n">
         <v>-0.0002</v>
@@ -3163,31 +3163,31 @@
         <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="M51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="N51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="O51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="P51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="Q51" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
     </row>
     <row r="52">
@@ -3216,31 +3216,31 @@
         <v>-0.014</v>
       </c>
       <c r="I52" t="n">
-        <v>-0.0142</v>
+        <v>-0.0175</v>
       </c>
       <c r="J52" t="n">
-        <v>-0.0146</v>
+        <v>-0.0179</v>
       </c>
       <c r="K52" t="n">
-        <v>-0.0149</v>
+        <v>-0.0181</v>
       </c>
       <c r="L52" t="n">
-        <v>-0.0035</v>
+        <v>-0.0071</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.0026</v>
+        <v>-0.003</v>
       </c>
       <c r="N52" t="n">
-        <v>-0.0017</v>
+        <v>-0.0021</v>
       </c>
       <c r="O52" t="n">
-        <v>-0.0009</v>
+        <v>-0.0012</v>
       </c>
       <c r="P52" t="n">
-        <v>0.0012</v>
+        <v>0.0015</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.0011</v>
+        <v>0.0013</v>
       </c>
     </row>
     <row r="53">
@@ -3269,28 +3269,28 @@
         <v>0.0338</v>
       </c>
       <c r="I53" t="n">
-        <v>0.0333</v>
+        <v>0.0389</v>
       </c>
       <c r="J53" t="n">
-        <v>0.0165</v>
+        <v>0.022</v>
       </c>
       <c r="K53" t="n">
-        <v>0.0162</v>
+        <v>0.019</v>
       </c>
       <c r="L53" t="n">
-        <v>0.0161</v>
+        <v>0.0188</v>
       </c>
       <c r="M53" t="n">
-        <v>0.0159</v>
+        <v>0.0186</v>
       </c>
       <c r="N53" t="n">
-        <v>0.0158</v>
+        <v>0.0184</v>
       </c>
       <c r="O53" t="n">
-        <v>0.0156</v>
+        <v>0.0183</v>
       </c>
       <c r="P53" t="n">
-        <v>0.0001</v>
+        <v>0.0027</v>
       </c>
       <c r="Q53" t="n">
         <v>0</v>

</xml_diff>